<commit_message>
Analiza 2 kazalcev, poprava tabel
</commit_message>
<xml_diff>
--- a/Data-Adidas/IPI_adidas.xlsx
+++ b/Data-Adidas/IPI_adidas.xlsx
@@ -24,12 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Exchange rate: EUR/USD</t>
-  </si>
-  <si>
-    <t>Operating revenue (Turnover)</t>
   </si>
   <si>
     <t>Sales</t>
@@ -451,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,24 +498,24 @@
         <v>1.0887</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="6">
-        <v>26787469.511628199</v>
+        <v>26557172.541618299</v>
       </c>
       <c r="C3" s="6">
-        <v>25285047.7412939</v>
+        <v>25092687.644362401</v>
       </c>
       <c r="D3" s="6">
-        <v>25601448.004007298</v>
+        <v>25446738.358974501</v>
       </c>
       <c r="E3" s="6">
-        <v>20725705.5444717</v>
+        <v>20334634.607791901</v>
       </c>
       <c r="F3" s="9">
-        <v>18823621.9084263</v>
+        <v>18588462.722063102</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -526,19 +523,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="6">
-        <v>26557172.541618299</v>
+        <v>11415989.313363999</v>
       </c>
       <c r="C4" s="6">
-        <v>25092687.644362401</v>
+        <v>11522140.8060789</v>
       </c>
       <c r="D4" s="6">
-        <v>25446738.358974501</v>
+        <v>12048163.519382499</v>
       </c>
       <c r="E4" s="6">
-        <v>20334634.607791901</v>
+        <v>10033973.709583299</v>
       </c>
       <c r="F4" s="9">
-        <v>18588462.722063102</v>
+        <v>9134192.4703121204</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -546,59 +543,59 @@
         <v>3</v>
       </c>
       <c r="B5" s="6">
-        <v>11415989.313363999</v>
+        <v>15371480.1982641</v>
       </c>
       <c r="C5" s="6">
-        <v>11522140.8060789</v>
+        <v>13762906.935215</v>
       </c>
       <c r="D5" s="6">
-        <v>12048163.519382499</v>
+        <v>13553284.4846249</v>
       </c>
       <c r="E5" s="6">
-        <v>10033973.709583299</v>
+        <v>10691731.834888499</v>
       </c>
       <c r="F5" s="9">
-        <v>9134192.4703121204</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9689429.43811417</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="6">
-        <v>15371480.1982641</v>
+        <v>12368632.389307</v>
       </c>
       <c r="C6" s="6">
-        <v>13762906.935215</v>
+        <v>11062995.5747128</v>
       </c>
       <c r="D6" s="6">
-        <v>13553284.4846249</v>
+        <v>11074332.265377</v>
       </c>
       <c r="E6" s="6">
-        <v>10691731.834888499</v>
+        <v>9124285.7894897498</v>
       </c>
       <c r="F6" s="9">
-        <v>9689429.43811417</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+        <v>8550649.3041515406</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="6">
-        <v>12368632.389307</v>
+        <v>3002847.8089570999</v>
       </c>
       <c r="C7" s="6">
-        <v>11062995.5747128</v>
+        <v>2699911.3605022398</v>
       </c>
       <c r="D7" s="6">
-        <v>11074332.265377</v>
+        <v>2478952.2192478199</v>
       </c>
       <c r="E7" s="6">
-        <v>9124285.7894897498</v>
+        <v>1567446.0453987101</v>
       </c>
       <c r="F7" s="9">
-        <v>8550649.3041515406</v>
+        <v>1138780.1339626301</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -606,19 +603,19 @@
         <v>6</v>
       </c>
       <c r="B8" s="6">
-        <v>3002847.8089570999</v>
+        <v>56169.992685318</v>
       </c>
       <c r="C8" s="6">
-        <v>2699911.3605022398</v>
+        <v>27480.0138473511</v>
       </c>
       <c r="D8" s="6">
-        <v>2478952.2192478199</v>
+        <v>29982.4893474579</v>
       </c>
       <c r="E8" s="6">
-        <v>1567446.0453987101</v>
+        <v>22136.090755462599</v>
       </c>
       <c r="F8" s="9">
-        <v>1138780.1339626301</v>
+        <v>21773.998737335201</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -626,19 +623,19 @@
         <v>7</v>
       </c>
       <c r="B9" s="6">
-        <v>56169.992685318</v>
+        <v>185360.975861549</v>
       </c>
       <c r="C9" s="6">
-        <v>27480.0138473511</v>
+        <v>4580.0023078918503</v>
       </c>
       <c r="D9" s="6">
-        <v>29982.4893474579</v>
+        <v>83950.970172882095</v>
       </c>
       <c r="E9" s="6">
-        <v>22136.090755462599</v>
+        <v>67462.371826171904</v>
       </c>
       <c r="F9" s="9">
-        <v>21773.998737335201</v>
+        <v>87095.994949340806</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -646,19 +643,19 @@
         <v>8</v>
       </c>
       <c r="B10" s="6">
-        <v>185360.975861549</v>
+        <v>2873656.8257808699</v>
       </c>
       <c r="C10" s="6">
-        <v>4580.0023078918503</v>
+        <v>2722811.3720416999</v>
       </c>
       <c r="D10" s="6">
-        <v>83950.970172882095</v>
+        <v>2424983.7384223901</v>
       </c>
       <c r="E10" s="6">
-        <v>67462.371826171904</v>
+        <v>1522119.7643279999</v>
       </c>
       <c r="F10" s="9">
-        <v>87095.994949340806</v>
+        <v>1073458.13775063</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -666,19 +663,19 @@
         <v>9</v>
       </c>
       <c r="B11" s="6">
-        <v>2873656.8257808699</v>
+        <v>720099.30622577702</v>
       </c>
       <c r="C11" s="6">
-        <v>2722811.3720416999</v>
+        <v>766005.38599491096</v>
       </c>
       <c r="D11" s="6">
-        <v>2424983.7384223901</v>
+        <v>801132.11536407506</v>
       </c>
       <c r="E11" s="6">
-        <v>1522119.7643279999</v>
+        <v>447992.31290817301</v>
       </c>
       <c r="F11" s="9">
-        <v>1073458.13775063</v>
+        <v>376690.17815589899</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -686,19 +683,19 @@
         <v>10</v>
       </c>
       <c r="B12" s="6">
-        <v>720099.30622577702</v>
+        <v>2153557.51955509</v>
       </c>
       <c r="C12" s="6">
-        <v>766005.38599491096</v>
+        <v>1956805.9860467899</v>
       </c>
       <c r="D12" s="6">
-        <v>801132.11536407506</v>
+        <v>1623851.62305832</v>
       </c>
       <c r="E12" s="6">
-        <v>447992.31290817301</v>
+        <v>1074127.4514198301</v>
       </c>
       <c r="F12" s="9">
-        <v>376690.17815589899</v>
+        <v>696767.95959472703</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -706,58 +703,38 @@
         <v>11</v>
       </c>
       <c r="B13" s="6">
-        <v>2153557.51955509</v>
+        <v>64033.791661262498</v>
       </c>
       <c r="C13" s="6">
-        <v>1956805.9860467899</v>
+        <v>-9160.0046157836896</v>
       </c>
       <c r="D13" s="6">
-        <v>1623851.62305832</v>
+        <v>-308219.99049186701</v>
       </c>
       <c r="E13" s="6">
-        <v>1074127.4514198301</v>
+        <v>-1054.0995597839401</v>
       </c>
       <c r="F13" s="9">
-        <v>696767.95959472703</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>-6532.1996212005597</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="6">
-        <v>64033.791661262498</v>
+        <v>2217591.3112163502</v>
       </c>
       <c r="C14" s="6">
-        <v>-9160.0046157836896</v>
+        <v>1947645.9814310099</v>
       </c>
       <c r="D14" s="6">
-        <v>-308219.99049186701</v>
+        <v>1315631.6325664499</v>
       </c>
       <c r="E14" s="6">
-        <v>-1054.0995597839401</v>
+        <v>1073073.3518600501</v>
       </c>
       <c r="F14" s="9">
-        <v>-6532.1996212005597</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="6">
-        <v>2217591.3112163502</v>
-      </c>
-      <c r="C15" s="6">
-        <v>1947645.9814310099</v>
-      </c>
-      <c r="D15" s="6">
-        <v>1315631.6325664499</v>
-      </c>
-      <c r="E15" s="6">
-        <v>1073073.3518600501</v>
-      </c>
-      <c r="F15" s="9">
         <v>690235.759973526</v>
       </c>
     </row>

</xml_diff>